<commit_message>
shedule and leaderboard done for badminton and volleyball
</commit_message>
<xml_diff>
--- a/Backend/data/GC_TEST.xlsx
+++ b/Backend/data/GC_TEST.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GC WEB\Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE96125-BF6E-4A99-8EA4-AF1B0746892B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF06B386-1D13-4822-A4EC-BC586CF75DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{19AC486F-21D9-43D7-A072-27F5986CB41D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{19AC486F-21D9-43D7-A072-27F5986CB41D}"/>
   </bookViews>
   <sheets>
-    <sheet name="VB_MEN_SCHEDULE" sheetId="1" r:id="rId1"/>
-    <sheet name="VB_MEN_LEADERBOARD" sheetId="5" r:id="rId2"/>
-    <sheet name="VB_WOMEN_SCHEDULE" sheetId="3" r:id="rId3"/>
-    <sheet name="VB_WOMEN_LEADERBOARD" sheetId="6" r:id="rId4"/>
+    <sheet name="BT_MEN_SCHEDULE" sheetId="7" r:id="rId1"/>
+    <sheet name="BT_MEN_LEADERBOARD" sheetId="13" r:id="rId2"/>
+    <sheet name="BT_WOMEN_SCHEDULE" sheetId="9" r:id="rId3"/>
+    <sheet name="BT_WOMEN_LEADERBOARD" sheetId="11" r:id="rId4"/>
+    <sheet name="VB_MEN_SCHEDULE" sheetId="1" r:id="rId5"/>
+    <sheet name="VB_MEN_LEADERBOARD" sheetId="5" r:id="rId6"/>
+    <sheet name="VB_WOMEN_SCHEDULE" sheetId="3" r:id="rId7"/>
+    <sheet name="VB_WOMEN_LEADERBOARD" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="118">
   <si>
     <t>VOLLEYBALL - MEN</t>
   </si>
@@ -250,6 +254,147 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>BADMINTON(MEN)</t>
+  </si>
+  <si>
+    <t>Majestic Eagles</t>
+  </si>
+  <si>
+    <t>5:15pm - 7:15pm</t>
+  </si>
+  <si>
+    <t>Agora Auditorium</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>6:45am - 8:45am</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>Ferocious Tigers</t>
+  </si>
+  <si>
+    <t>9:00am - 11:00am</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>7am - 9:00am</t>
+  </si>
+  <si>
+    <t>10:35am - 12:35pm</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2:15pm - 4:15pm</t>
+  </si>
+  <si>
+    <t>5:50pm - 7:50pm</t>
+  </si>
+  <si>
+    <t>3-0</t>
+  </si>
+  <si>
+    <t>Pool A Winner   (Rhinos)</t>
+  </si>
+  <si>
+    <t>Pool B Runner Up (WILD WOLVES)</t>
+  </si>
+  <si>
+    <t>Pool B Winner    (Sharks)</t>
+  </si>
+  <si>
+    <t>Pool A Runner Up (Lions)</t>
+  </si>
+  <si>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>9am - 11:00pm</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>POINTS</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>BADMINTON(WOMEN)</t>
+  </si>
+  <si>
+    <t>Stealthy panthers</t>
+  </si>
+  <si>
+    <t>BYE</t>
+  </si>
+  <si>
+    <t>4:30pm - 5:45pm</t>
+  </si>
+  <si>
+    <t>Starwart Rhinos</t>
+  </si>
+  <si>
+    <t>12:40pm - 1:55pm</t>
+  </si>
+  <si>
+    <t>9:15am - 10:30am</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>12:50pm - 2:05pm</t>
+  </si>
+  <si>
+    <t>8:05pm - 9:20pm</t>
+  </si>
+  <si>
+    <t>Pool A Winner   (MIGHTY LIONS)</t>
+  </si>
+  <si>
+    <t>Pool B Runner Up  (SAVAGE SHARKS)</t>
+  </si>
+  <si>
+    <t>9:00am - 10:15am</t>
+  </si>
+  <si>
+    <t>Pool B Winner    (STALWART RHINOS)</t>
+  </si>
+  <si>
+    <t>Pool A Runner Up (STEALTHY PANTHERS)</t>
+  </si>
+  <si>
+    <t>1:50am - 2:05pm</t>
+  </si>
+  <si>
+    <t>Savage sharks</t>
+  </si>
+  <si>
+    <t>11am - 12:00pm</t>
   </si>
 </sst>
 </file>
@@ -262,7 +407,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +452,14 @@
       <color theme="1"/>
       <name val="EB Garamond"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +488,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8AF"/>
+        <bgColor rgb="FFE6B8AF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -546,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -692,29 +861,115 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,11 +1283,3724 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C362980-9BF9-4606-B327-EBFA27878502}">
+  <dimension ref="A1:P1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.21875" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" customWidth="1"/>
+    <col min="9" max="9" width="33.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:16" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="10">
+        <v>45716</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="81"/>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="13">
+        <v>45717</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="27"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="39"/>
+    </row>
+    <row r="5" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="81"/>
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="13">
+        <v>45717</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="81"/>
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="10">
+        <v>45717</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="81"/>
+      <c r="B7" s="7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="10">
+        <v>45718</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:16" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="81"/>
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="13">
+        <v>45718</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="81"/>
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="13">
+        <v>45718</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:16" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="81"/>
+      <c r="B10" s="7">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="10">
+        <v>45718</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="81"/>
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="10">
+        <v>45719</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="15">
+        <v>45691</v>
+      </c>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="81"/>
+      <c r="B12" s="7">
+        <v>10</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="10">
+        <v>45720</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="81"/>
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="13">
+        <v>45721</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="53">
+        <v>45717</v>
+      </c>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="82"/>
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="13">
+        <v>45723</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="83"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="54">
+        <v>45724</v>
+      </c>
+      <c r="G16" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="56"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="82"/>
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="54">
+        <v>45724</v>
+      </c>
+      <c r="G17" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="56"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="83"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="54">
+        <v>45724</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="56"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="83"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="54">
+        <v>45725</v>
+      </c>
+      <c r="G21" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="56"/>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="182" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:I18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4633AB12-74C1-47B3-9014-BB0E624802F2}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="58">
+        <v>3</v>
+      </c>
+      <c r="D2" s="58">
+        <v>3</v>
+      </c>
+      <c r="E2" s="58">
+        <v>0</v>
+      </c>
+      <c r="F2" s="58">
+        <v>6</v>
+      </c>
+      <c r="G2" s="58">
+        <v>9</v>
+      </c>
+      <c r="H2" s="58">
+        <v>3</v>
+      </c>
+      <c r="I2" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="58">
+        <v>3</v>
+      </c>
+      <c r="D3" s="58">
+        <v>1</v>
+      </c>
+      <c r="E3" s="58">
+        <v>2</v>
+      </c>
+      <c r="F3" s="58">
+        <v>2</v>
+      </c>
+      <c r="G3" s="58">
+        <v>7</v>
+      </c>
+      <c r="H3" s="58">
+        <v>6</v>
+      </c>
+      <c r="I3" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="62">
+        <v>3</v>
+      </c>
+      <c r="D4" s="62">
+        <v>0</v>
+      </c>
+      <c r="E4" s="62">
+        <v>3</v>
+      </c>
+      <c r="F4" s="62">
+        <v>0</v>
+      </c>
+      <c r="G4" s="62">
+        <v>0</v>
+      </c>
+      <c r="H4" s="62">
+        <v>9</v>
+      </c>
+      <c r="I4" s="63">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="64">
+        <v>3</v>
+      </c>
+      <c r="D5" s="62">
+        <v>2</v>
+      </c>
+      <c r="E5" s="62">
+        <v>1</v>
+      </c>
+      <c r="F5" s="62">
+        <v>4</v>
+      </c>
+      <c r="G5" s="62">
+        <v>7</v>
+      </c>
+      <c r="H5" s="62">
+        <v>5</v>
+      </c>
+      <c r="I5" s="63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="58">
+        <v>3</v>
+      </c>
+      <c r="D7" s="58">
+        <v>0</v>
+      </c>
+      <c r="E7" s="58">
+        <v>3</v>
+      </c>
+      <c r="F7" s="58">
+        <v>0</v>
+      </c>
+      <c r="G7" s="58">
+        <v>4</v>
+      </c>
+      <c r="H7" s="58">
+        <v>9</v>
+      </c>
+      <c r="I7" s="61">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="58">
+        <v>3</v>
+      </c>
+      <c r="D8" s="58">
+        <v>3</v>
+      </c>
+      <c r="E8" s="58">
+        <v>0</v>
+      </c>
+      <c r="F8" s="58">
+        <v>6</v>
+      </c>
+      <c r="G8" s="58">
+        <v>9</v>
+      </c>
+      <c r="H8" s="58">
+        <v>3</v>
+      </c>
+      <c r="I8" s="58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="62">
+        <v>2</v>
+      </c>
+      <c r="D9" s="62">
+        <v>1</v>
+      </c>
+      <c r="E9" s="62">
+        <v>1</v>
+      </c>
+      <c r="F9" s="62">
+        <v>2</v>
+      </c>
+      <c r="G9" s="62">
+        <v>3</v>
+      </c>
+      <c r="H9" s="62">
+        <v>5</v>
+      </c>
+      <c r="I9" s="62">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="62">
+        <v>2</v>
+      </c>
+      <c r="D10" s="62">
+        <v>1</v>
+      </c>
+      <c r="E10" s="62">
+        <v>1</v>
+      </c>
+      <c r="F10" s="62">
+        <v>2</v>
+      </c>
+      <c r="G10" s="62">
+        <v>5</v>
+      </c>
+      <c r="H10" s="62">
+        <v>4</v>
+      </c>
+      <c r="I10" s="62">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAF3DED-7C04-475E-982A-1D5DCD3C36AA}">
+  <dimension ref="A1:L1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="4.21875" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="39.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" customWidth="1"/>
+    <col min="9" max="9" width="33.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="77" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:12" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="10">
+        <v>45716</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="27"/>
+      <c r="L3" s="65"/>
+    </row>
+    <row r="4" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="81"/>
+      <c r="B4" s="66">
+        <v>2</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="67">
+        <v>45717</v>
+      </c>
+      <c r="G4" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="68"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+    </row>
+    <row r="5" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="81"/>
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="13">
+        <v>45717</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+    </row>
+    <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="81"/>
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="13">
+        <v>45723</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+    </row>
+    <row r="7" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="81"/>
+      <c r="B7" s="7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="10">
+        <v>45718</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="81"/>
+      <c r="B8" s="66">
+        <v>6</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="67">
+        <v>45718</v>
+      </c>
+      <c r="G8" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="68"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="81"/>
+      <c r="B9" s="69">
+        <v>7</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="70">
+        <v>45718</v>
+      </c>
+      <c r="G9" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="50"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="81"/>
+      <c r="B10" s="12">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="13">
+        <v>45719</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="81"/>
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="10">
+        <v>45720</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="27"/>
+      <c r="K11" s="71"/>
+    </row>
+    <row r="12" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="81"/>
+      <c r="B12" s="66">
+        <v>10</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="67">
+        <v>45721</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="72"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="81"/>
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="13">
+        <v>45722</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="82"/>
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="13">
+        <v>45718</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="83"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="54">
+        <v>45724</v>
+      </c>
+      <c r="G16" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="56"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="82"/>
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="54">
+        <v>45724</v>
+      </c>
+      <c r="G17" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="56"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="83"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="54">
+        <v>45724</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="56"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="83"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="54">
+        <v>45725</v>
+      </c>
+      <c r="G21" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="56"/>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="182" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:I18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024EE61C-0112-451F-A67F-ED7F0B9161D9}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="58">
+        <v>2</v>
+      </c>
+      <c r="D2" s="58">
+        <v>0</v>
+      </c>
+      <c r="E2" s="58">
+        <v>2</v>
+      </c>
+      <c r="F2" s="58">
+        <v>0</v>
+      </c>
+      <c r="G2" s="58">
+        <v>0</v>
+      </c>
+      <c r="H2" s="58">
+        <v>4</v>
+      </c>
+      <c r="I2" s="59">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="74">
+        <v>2</v>
+      </c>
+      <c r="D3" s="75">
+        <v>1</v>
+      </c>
+      <c r="E3" s="74">
+        <v>1</v>
+      </c>
+      <c r="F3" s="75">
+        <v>2</v>
+      </c>
+      <c r="G3" s="75">
+        <v>2</v>
+      </c>
+      <c r="H3" s="74">
+        <v>2</v>
+      </c>
+      <c r="I3" s="76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="74">
+        <v>2</v>
+      </c>
+      <c r="D4" s="74">
+        <v>2</v>
+      </c>
+      <c r="E4" s="75">
+        <v>0</v>
+      </c>
+      <c r="F4" s="74">
+        <v>4</v>
+      </c>
+      <c r="G4" s="74">
+        <v>2</v>
+      </c>
+      <c r="H4" s="75">
+        <v>0</v>
+      </c>
+      <c r="I4" s="76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="58">
+        <v>1</v>
+      </c>
+      <c r="D5" s="58">
+        <v>0</v>
+      </c>
+      <c r="E5" s="58">
+        <v>1</v>
+      </c>
+      <c r="F5" s="58">
+        <v>0</v>
+      </c>
+      <c r="G5" s="58">
+        <v>0</v>
+      </c>
+      <c r="H5" s="58">
+        <v>2</v>
+      </c>
+      <c r="I5" s="61">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="58">
+        <v>3</v>
+      </c>
+      <c r="D6" s="58">
+        <v>3</v>
+      </c>
+      <c r="E6" s="58">
+        <v>0</v>
+      </c>
+      <c r="F6" s="58">
+        <v>6</v>
+      </c>
+      <c r="G6" s="58">
+        <v>6</v>
+      </c>
+      <c r="H6" s="58">
+        <v>0</v>
+      </c>
+      <c r="I6" s="58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="62">
+        <v>2</v>
+      </c>
+      <c r="D7" s="62">
+        <v>1</v>
+      </c>
+      <c r="E7" s="62">
+        <v>1</v>
+      </c>
+      <c r="F7" s="62">
+        <v>2</v>
+      </c>
+      <c r="G7" s="62">
+        <v>2</v>
+      </c>
+      <c r="H7" s="62">
+        <v>3</v>
+      </c>
+      <c r="I7" s="62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="62">
+        <v>2</v>
+      </c>
+      <c r="D8" s="62">
+        <v>0</v>
+      </c>
+      <c r="E8" s="62">
+        <v>2</v>
+      </c>
+      <c r="F8" s="62">
+        <v>0</v>
+      </c>
+      <c r="G8" s="62">
+        <v>1</v>
+      </c>
+      <c r="H8" s="62">
+        <v>4</v>
+      </c>
+      <c r="I8" s="62">
+        <v>-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CF8DC9-CBCD-437D-8122-8FD8CCAFA831}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="50" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,18 +5015,18 @@
     <col min="9" max="9" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:9" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" ht="123" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -1088,7 +5056,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="86" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -1117,7 +5085,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -1144,7 +5112,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="53"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -1171,7 +5139,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -1198,7 +5166,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -1225,7 +5193,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="12">
         <v>6</v>
       </c>
@@ -1252,7 +5220,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -1279,7 +5247,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="53"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -1306,7 +5274,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
+      <c r="A11" s="81"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -1333,7 +5301,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -1358,7 +5326,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="53"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -1383,7 +5351,7 @@
       <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
+      <c r="A14" s="82"/>
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -1416,12 +5384,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFEAF12-B892-45FF-BB3F-D7F1C442F987}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView topLeftCell="N1" zoomScale="82" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,12 +5698,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AFEC59-8DD1-4B82-A602-CD123E215FCB}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1752,17 +5720,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
@@ -1794,7 +5762,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="84" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="32">
@@ -1824,7 +5792,7 @@
       <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="36">
         <v>2</v>
       </c>
@@ -1853,7 +5821,7 @@
       <c r="K4" s="39"/>
     </row>
     <row r="5" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="36">
         <v>3</v>
       </c>
@@ -1881,7 +5849,7 @@
       <c r="J5" s="27"/>
     </row>
     <row r="6" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="56"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="32">
         <v>4</v>
       </c>
@@ -1909,7 +5877,7 @@
       <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="56"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="36">
         <v>5</v>
       </c>
@@ -1937,7 +5905,7 @@
       <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="57"/>
+      <c r="A8" s="85"/>
       <c r="B8" s="32">
         <v>6</v>
       </c>
@@ -2034,19 +6002,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="60"/>
+      <c r="A15" s="89"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="91"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="86" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -2074,7 +6042,7 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A17" s="54"/>
+      <c r="A17" s="82"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -2100,15 +6068,15 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="61"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="51"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="79"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2140,15 +6108,15 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="61"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="79"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3182,12 +7150,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878C0A0D-E4CD-4971-9A03-4D421A3D28C8}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3286,7 +7254,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="45">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated api link and styles for schedule and leaderboard
</commit_message>
<xml_diff>
--- a/Backend/data/GC_TEST.xlsx
+++ b/Backend/data/GC_TEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GC WEB\Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31F1451-4083-46A2-AF93-453926820FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE593259-74D7-4565-865D-EDC10595373C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="17" activeTab="19" xr2:uid="{19AC486F-21D9-43D7-A072-27F5986CB41D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="12" xr2:uid="{19AC486F-21D9-43D7-A072-27F5986CB41D}"/>
   </bookViews>
   <sheets>
     <sheet name="AT_ALL_SCHEDULE" sheetId="35" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="414">
   <si>
     <t>VOLLEYBALL - MEN</t>
   </si>
@@ -1312,6 +1312,9 @@
   </si>
   <si>
     <t>TigersSSSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PANTHERS (BTECH B22)</t>
   </si>
 </sst>
 </file>
@@ -2569,21 +2572,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2596,17 +2594,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2614,51 +2620,40 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2668,6 +2663,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3097,261 +3100,261 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="166" t="s">
         <v>278</v>
       </c>
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="166" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="183">
+      <c r="C2" s="169">
         <v>45716</v>
       </c>
-      <c r="D2" s="173" t="s">
+      <c r="D2" s="166" t="s">
         <v>280</v>
       </c>
-      <c r="E2" s="173" t="s">
+      <c r="E2" s="166" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="183">
+      <c r="F2" s="169">
         <v>45716</v>
       </c>
-      <c r="G2" s="173" t="s">
+      <c r="G2" s="166" t="s">
         <v>281</v>
       </c>
-      <c r="H2" s="173" t="s">
+      <c r="H2" s="166" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="171"/>
-      <c r="B3" s="171"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
+      <c r="A3" s="167"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="171"/>
-      <c r="B4" s="171"/>
-      <c r="C4" s="171"/>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
+      <c r="A4" s="167"/>
+      <c r="B4" s="167"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
-      <c r="B5" s="172"/>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="172"/>
-      <c r="H5" s="172"/>
+      <c r="A5" s="167"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="168"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="168"/>
+      <c r="H5" s="168"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="171"/>
-      <c r="B6" s="173" t="s">
+      <c r="A6" s="167"/>
+      <c r="B6" s="166" t="s">
         <v>282</v>
       </c>
-      <c r="C6" s="183">
+      <c r="C6" s="169">
         <v>45719</v>
       </c>
-      <c r="D6" s="173" t="s">
+      <c r="D6" s="166" t="s">
         <v>283</v>
       </c>
-      <c r="E6" s="173" t="s">
+      <c r="E6" s="166" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="183">
+      <c r="F6" s="169">
         <v>45719</v>
       </c>
-      <c r="G6" s="173" t="s">
+      <c r="G6" s="166" t="s">
         <v>284</v>
       </c>
-      <c r="H6" s="173" t="s">
+      <c r="H6" s="166" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="171"/>
-      <c r="B7" s="171"/>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="171"/>
-      <c r="H7" s="171"/>
+      <c r="A7" s="167"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
+      <c r="E7" s="167"/>
+      <c r="F7" s="167"/>
+      <c r="G7" s="167"/>
+      <c r="H7" s="167"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="171"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="171"/>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
+      <c r="A8" s="167"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="167"/>
+      <c r="E8" s="167"/>
+      <c r="F8" s="167"/>
+      <c r="G8" s="167"/>
+      <c r="H8" s="167"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
-      <c r="B9" s="172"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="172"/>
-      <c r="G9" s="172"/>
-      <c r="H9" s="172"/>
+      <c r="A9" s="167"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="168"/>
+      <c r="D9" s="168"/>
+      <c r="E9" s="168"/>
+      <c r="F9" s="168"/>
+      <c r="G9" s="168"/>
+      <c r="H9" s="168"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="171"/>
-      <c r="B10" s="173" t="s">
+      <c r="A10" s="167"/>
+      <c r="B10" s="166" t="s">
         <v>285</v>
       </c>
-      <c r="C10" s="183">
+      <c r="C10" s="169">
         <v>45720</v>
       </c>
-      <c r="D10" s="173" t="s">
+      <c r="D10" s="166" t="s">
         <v>283</v>
       </c>
-      <c r="E10" s="173" t="s">
+      <c r="E10" s="166" t="s">
         <v>170</v>
       </c>
-      <c r="F10" s="183">
+      <c r="F10" s="169">
         <v>45720</v>
       </c>
-      <c r="G10" s="173" t="s">
+      <c r="G10" s="166" t="s">
         <v>284</v>
       </c>
-      <c r="H10" s="173" t="s">
+      <c r="H10" s="166" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="171"/>
-      <c r="B11" s="171"/>
-      <c r="C11" s="171"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="171"/>
-      <c r="F11" s="171"/>
-      <c r="G11" s="171"/>
-      <c r="H11" s="171"/>
+      <c r="A11" s="167"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="167"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="171"/>
-      <c r="B12" s="171"/>
-      <c r="C12" s="171"/>
-      <c r="D12" s="171"/>
-      <c r="E12" s="171"/>
-      <c r="F12" s="171"/>
-      <c r="G12" s="171"/>
-      <c r="H12" s="171"/>
+      <c r="A12" s="167"/>
+      <c r="B12" s="167"/>
+      <c r="C12" s="167"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="167"/>
+      <c r="F12" s="167"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="167"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="171"/>
-      <c r="B13" s="172"/>
-      <c r="C13" s="172"/>
-      <c r="D13" s="172"/>
-      <c r="E13" s="172"/>
-      <c r="F13" s="172"/>
-      <c r="G13" s="172"/>
-      <c r="H13" s="172"/>
+      <c r="A13" s="167"/>
+      <c r="B13" s="168"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="168"/>
+      <c r="E13" s="168"/>
+      <c r="F13" s="168"/>
+      <c r="G13" s="168"/>
+      <c r="H13" s="168"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="171"/>
-      <c r="B14" s="173" t="s">
+      <c r="A14" s="167"/>
+      <c r="B14" s="166" t="s">
         <v>286</v>
       </c>
-      <c r="C14" s="183">
+      <c r="C14" s="169">
         <v>45722</v>
       </c>
-      <c r="D14" s="173" t="s">
+      <c r="D14" s="166" t="s">
         <v>283</v>
       </c>
-      <c r="E14" s="186" t="s">
+      <c r="E14" s="170" t="s">
         <v>170</v>
       </c>
-      <c r="F14" s="183">
+      <c r="F14" s="169">
         <v>45722</v>
       </c>
-      <c r="G14" s="173" t="s">
+      <c r="G14" s="166" t="s">
         <v>284</v>
       </c>
-      <c r="H14" s="186" t="s">
+      <c r="H14" s="170" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="171"/>
-      <c r="B15" s="172"/>
-      <c r="C15" s="172"/>
-      <c r="D15" s="172"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="172"/>
-      <c r="G15" s="172"/>
-      <c r="H15" s="172"/>
+      <c r="A15" s="167"/>
+      <c r="B15" s="168"/>
+      <c r="C15" s="168"/>
+      <c r="D15" s="168"/>
+      <c r="E15" s="168"/>
+      <c r="F15" s="168"/>
+      <c r="G15" s="168"/>
+      <c r="H15" s="168"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="171"/>
-      <c r="B16" s="173" t="s">
+      <c r="A16" s="167"/>
+      <c r="B16" s="166" t="s">
         <v>287</v>
       </c>
-      <c r="C16" s="183">
+      <c r="C16" s="169">
         <v>45723</v>
       </c>
-      <c r="D16" s="173" t="s">
+      <c r="D16" s="166" t="s">
         <v>283</v>
       </c>
-      <c r="E16" s="173" t="s">
+      <c r="E16" s="166" t="s">
         <v>170</v>
       </c>
-      <c r="F16" s="184"/>
-      <c r="G16" s="175"/>
-      <c r="H16" s="176"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="172"/>
+      <c r="H16" s="173"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="171"/>
-      <c r="B17" s="171"/>
-      <c r="C17" s="171"/>
-      <c r="D17" s="171"/>
-      <c r="E17" s="171"/>
-      <c r="F17" s="177"/>
-      <c r="G17" s="178"/>
-      <c r="H17" s="179"/>
+      <c r="A17" s="167"/>
+      <c r="B17" s="167"/>
+      <c r="C17" s="167"/>
+      <c r="D17" s="167"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="174"/>
+      <c r="G17" s="175"/>
+      <c r="H17" s="176"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="171"/>
-      <c r="B18" s="171"/>
-      <c r="C18" s="171"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="171"/>
-      <c r="F18" s="177"/>
-      <c r="G18" s="178"/>
-      <c r="H18" s="179"/>
+      <c r="A18" s="167"/>
+      <c r="B18" s="167"/>
+      <c r="C18" s="167"/>
+      <c r="D18" s="167"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="175"/>
+      <c r="H18" s="176"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="172"/>
-      <c r="B19" s="172"/>
-      <c r="C19" s="172"/>
-      <c r="D19" s="172"/>
-      <c r="E19" s="172"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="181"/>
-      <c r="H19" s="182"/>
+      <c r="A19" s="168"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="168"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="168"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="178"/>
+      <c r="H19" s="179"/>
     </row>
     <row r="20" spans="1:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="184"/>
-      <c r="D20" s="175"/>
-      <c r="E20" s="175"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="175"/>
-      <c r="H20" s="176"/>
+      <c r="C20" s="180"/>
+      <c r="D20" s="172"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="172"/>
+      <c r="G20" s="172"/>
+      <c r="H20" s="173"/>
     </row>
     <row r="21" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="173" t="s">
+      <c r="A21" s="166" t="s">
         <v>288</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3377,7 +3380,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="171"/>
+      <c r="A22" s="167"/>
       <c r="B22" s="1" t="s">
         <v>282</v>
       </c>
@@ -3401,7 +3404,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="171"/>
+      <c r="A23" s="167"/>
       <c r="B23" s="1" t="s">
         <v>285</v>
       </c>
@@ -3425,7 +3428,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="171"/>
+      <c r="A24" s="167"/>
       <c r="B24" s="1" t="s">
         <v>287</v>
       </c>
@@ -3438,12 +3441,12 @@
       <c r="E24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="185"/>
-      <c r="G24" s="167"/>
-      <c r="H24" s="168"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="182"/>
+      <c r="H24" s="183"/>
     </row>
     <row r="25" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="171"/>
+      <c r="A25" s="167"/>
       <c r="B25" s="1" t="s">
         <v>286</v>
       </c>
@@ -3467,7 +3470,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="171"/>
+      <c r="A26" s="167"/>
       <c r="B26" s="1" t="s">
         <v>298</v>
       </c>
@@ -3480,12 +3483,12 @@
       <c r="E26" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F26" s="174"/>
-      <c r="G26" s="175"/>
-      <c r="H26" s="176"/>
+      <c r="F26" s="171"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="173"/>
     </row>
     <row r="27" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="171"/>
+      <c r="A27" s="167"/>
       <c r="B27" s="1" t="s">
         <v>300</v>
       </c>
@@ -3498,12 +3501,12 @@
       <c r="E27" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F27" s="177"/>
-      <c r="G27" s="178"/>
-      <c r="H27" s="179"/>
+      <c r="F27" s="174"/>
+      <c r="G27" s="175"/>
+      <c r="H27" s="176"/>
     </row>
     <row r="28" spans="1:8" ht="69" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="171"/>
+      <c r="A28" s="167"/>
       <c r="B28" s="1" t="s">
         <v>301</v>
       </c>
@@ -3516,12 +3519,12 @@
       <c r="E28" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F28" s="180"/>
-      <c r="G28" s="181"/>
-      <c r="H28" s="182"/>
+      <c r="F28" s="177"/>
+      <c r="G28" s="178"/>
+      <c r="H28" s="179"/>
     </row>
     <row r="29" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="171"/>
+      <c r="A29" s="167"/>
       <c r="B29" s="1" t="s">
         <v>302</v>
       </c>
@@ -3545,7 +3548,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="172"/>
+      <c r="A30" s="168"/>
       <c r="B30" s="1" t="s">
         <v>304</v>
       </c>
@@ -3564,28 +3567,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="A21:A30"/>
     <mergeCell ref="F26:H28"/>
@@ -3602,6 +3583,28 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="G6:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3889,17 +3892,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3931,7 +3934,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="170" t="s">
+      <c r="A3" s="193" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -3962,7 +3965,7 @@
       <c r="L3" s="65"/>
     </row>
     <row r="4" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="171"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="66">
         <v>2</v>
       </c>
@@ -3990,7 +3993,7 @@
       <c r="L4" s="65"/>
     </row>
     <row r="5" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -4020,7 +4023,7 @@
       <c r="L5" s="65"/>
     </row>
     <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="171"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -4050,7 +4053,7 @@
       <c r="L6" s="65"/>
     </row>
     <row r="7" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="171"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -4078,7 +4081,7 @@
       <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="171"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="66">
         <v>6</v>
       </c>
@@ -4104,7 +4107,7 @@
       <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="69">
         <v>7</v>
       </c>
@@ -4130,7 +4133,7 @@
       <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="171"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -4158,7 +4161,7 @@
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="171"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -4187,7 +4190,7 @@
       <c r="K11" s="71"/>
     </row>
     <row r="12" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="171"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="66">
         <v>10</v>
       </c>
@@ -4213,7 +4216,7 @@
       <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="171"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -4239,7 +4242,7 @@
       <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="172"/>
+      <c r="A14" s="168"/>
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -4267,19 +4270,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="166"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="168"/>
+      <c r="A15" s="190"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="193" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -4307,7 +4310,7 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -4333,15 +4336,15 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="166"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
+      <c r="A18" s="190"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4373,15 +4376,15 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="166"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
+      <c r="A20" s="190"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5706,15 +5709,15 @@
       <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="203"/>
-      <c r="B10" s="178"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="178"/>
-      <c r="E10" s="178"/>
-      <c r="F10" s="178"/>
-      <c r="G10" s="178"/>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
+      <c r="A10" s="196"/>
+      <c r="B10" s="175"/>
+      <c r="C10" s="175"/>
+      <c r="D10" s="175"/>
+      <c r="E10" s="175"/>
+      <c r="F10" s="175"/>
+      <c r="G10" s="175"/>
+      <c r="H10" s="175"/>
+      <c r="I10" s="175"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6724,8 +6727,8 @@
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6740,15 +6743,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="183"/>
       <c r="H1" s="104"/>
       <c r="I1" s="104"/>
     </row>
@@ -6782,7 +6785,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>198</v>
+        <v>413</v>
       </c>
       <c r="C3" s="105" t="s">
         <v>199</v>
@@ -7395,25 +7398,25 @@
       <c r="H30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="201"/>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
+      <c r="A31" s="199"/>
+      <c r="B31" s="182"/>
+      <c r="C31" s="182"/>
+      <c r="D31" s="182"/>
+      <c r="E31" s="182"/>
+      <c r="F31" s="182"/>
+      <c r="G31" s="183"/>
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="202" t="s">
+      <c r="A32" s="197" t="s">
         <v>209</v>
       </c>
-      <c r="B32" s="178"/>
-      <c r="C32" s="179"/>
-      <c r="D32" s="183"/>
+      <c r="B32" s="175"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="169"/>
       <c r="E32" s="198"/>
-      <c r="F32" s="173" t="s">
+      <c r="F32" s="166" t="s">
         <v>201</v>
       </c>
       <c r="G32" s="111"/>
@@ -7421,34 +7424,34 @@
       <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="177"/>
-      <c r="B33" s="178"/>
-      <c r="C33" s="179"/>
-      <c r="D33" s="171"/>
-      <c r="E33" s="171"/>
-      <c r="F33" s="171"/>
+      <c r="A33" s="174"/>
+      <c r="B33" s="175"/>
+      <c r="C33" s="176"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="167"/>
       <c r="G33" s="1"/>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
     </row>
     <row r="34" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="177"/>
-      <c r="B34" s="178"/>
-      <c r="C34" s="179"/>
-      <c r="D34" s="171"/>
-      <c r="E34" s="171"/>
-      <c r="F34" s="171"/>
+      <c r="A34" s="174"/>
+      <c r="B34" s="175"/>
+      <c r="C34" s="176"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
       <c r="G34" s="1"/>
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="180"/>
-      <c r="B35" s="181"/>
-      <c r="C35" s="182"/>
-      <c r="D35" s="172"/>
-      <c r="E35" s="172"/>
-      <c r="F35" s="172"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="178"/>
+      <c r="C35" s="179"/>
+      <c r="D35" s="168"/>
+      <c r="E35" s="168"/>
+      <c r="F35" s="168"/>
       <c r="G35" s="1"/>
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
@@ -8713,18 +8716,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="191" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="199"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
+      <c r="J1" s="200"/>
     </row>
     <row r="2" spans="1:14" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -8752,10 +8755,10 @@
       <c r="I2" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="178"/>
+      <c r="J2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="166" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -8782,13 +8785,13 @@
       <c r="I3" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="J3" s="178"/>
+      <c r="J3" s="175"/>
       <c r="L3" s="55"/>
       <c r="M3" s="55"/>
       <c r="N3" s="55"/>
     </row>
     <row r="4" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="171"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -8813,10 +8816,10 @@
       <c r="I4" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="J4" s="178"/>
+      <c r="J4" s="175"/>
     </row>
     <row r="5" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -8841,10 +8844,10 @@
       <c r="I5" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="J5" s="178"/>
+      <c r="J5" s="175"/>
     </row>
     <row r="6" spans="1:14" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="171"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -8869,10 +8872,10 @@
       <c r="I6" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="J6" s="178"/>
+      <c r="J6" s="175"/>
     </row>
     <row r="7" spans="1:14" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="171"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -8897,10 +8900,10 @@
       <c r="I7" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="J7" s="178"/>
+      <c r="J7" s="175"/>
     </row>
     <row r="8" spans="1:14" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="171"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -8925,10 +8928,10 @@
       <c r="I8" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="J8" s="178"/>
+      <c r="J8" s="175"/>
     </row>
     <row r="9" spans="1:14" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -8953,7 +8956,7 @@
       <c r="I9" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="178"/>
+      <c r="J9" s="175"/>
       <c r="L9" s="85" t="s">
         <v>123</v>
       </c>
@@ -8962,7 +8965,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="171"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -8987,7 +8990,7 @@
       <c r="I10" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="J10" s="178"/>
+      <c r="J10" s="175"/>
       <c r="L10" s="85" t="s">
         <v>125</v>
       </c>
@@ -8996,7 +8999,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="171"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -9021,10 +9024,10 @@
       <c r="I11" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="J11" s="178"/>
+      <c r="J11" s="175"/>
     </row>
     <row r="12" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="171"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -9047,10 +9050,10 @@
         <v>170</v>
       </c>
       <c r="I12" s="14"/>
-      <c r="J12" s="178"/>
+      <c r="J12" s="175"/>
     </row>
     <row r="13" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="171"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -9073,10 +9076,10 @@
         <v>170</v>
       </c>
       <c r="I13" s="11"/>
-      <c r="J13" s="178"/>
+      <c r="J13" s="175"/>
     </row>
     <row r="14" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="172"/>
+      <c r="A14" s="168"/>
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -9099,22 +9102,22 @@
         <v>170</v>
       </c>
       <c r="I14" s="14"/>
-      <c r="J14" s="178"/>
+      <c r="J14" s="175"/>
     </row>
     <row r="15" spans="1:14" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="193"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="168"/>
-      <c r="J15" s="178"/>
+      <c r="A15" s="201"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="175"/>
     </row>
     <row r="16" spans="1:14" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="166" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -9139,10 +9142,10 @@
         <v>170</v>
       </c>
       <c r="I16" s="56"/>
-      <c r="J16" s="178"/>
+      <c r="J16" s="175"/>
     </row>
     <row r="17" spans="1:10" ht="69" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1" t="s">
         <v>188</v>
       </c>
@@ -9165,19 +9168,19 @@
         <v>170</v>
       </c>
       <c r="I17" s="56"/>
-      <c r="J17" s="178"/>
+      <c r="J17" s="175"/>
     </row>
     <row r="18" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="193"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
-      <c r="J18" s="178"/>
+      <c r="A18" s="201"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
+      <c r="J18" s="175"/>
     </row>
     <row r="19" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -9205,19 +9208,19 @@
         <v>170</v>
       </c>
       <c r="I19" s="56"/>
-      <c r="J19" s="178"/>
+      <c r="J19" s="175"/>
     </row>
     <row r="20" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="193"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
-      <c r="J20" s="178"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="175"/>
     </row>
     <row r="21" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -9245,19 +9248,19 @@
         <v>170</v>
       </c>
       <c r="I21" s="56"/>
-      <c r="J21" s="178"/>
+      <c r="J21" s="175"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="199"/>
-      <c r="B22" s="178"/>
-      <c r="C22" s="178"/>
-      <c r="D22" s="178"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="178"/>
-      <c r="H22" s="178"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="178"/>
+      <c r="A22" s="200"/>
+      <c r="B22" s="175"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="175"/>
+      <c r="E22" s="175"/>
+      <c r="F22" s="175"/>
+      <c r="G22" s="175"/>
+      <c r="H22" s="175"/>
+      <c r="I22" s="175"/>
+      <c r="J22" s="175"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10564,18 +10567,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="199"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
+      <c r="J1" s="200"/>
     </row>
     <row r="2" spans="1:13" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -10603,10 +10606,10 @@
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="178"/>
+      <c r="J2" s="175"/>
     </row>
     <row r="3" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="166" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -10633,10 +10636,10 @@
       <c r="I3" s="15">
         <v>45689</v>
       </c>
-      <c r="J3" s="178"/>
+      <c r="J3" s="175"/>
     </row>
     <row r="4" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="171"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -10661,10 +10664,10 @@
       <c r="I4" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="J4" s="178"/>
+      <c r="J4" s="175"/>
     </row>
     <row r="5" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -10689,7 +10692,7 @@
       <c r="I5" s="53">
         <v>45661</v>
       </c>
-      <c r="J5" s="178"/>
+      <c r="J5" s="175"/>
       <c r="L5" s="85" t="s">
         <v>123</v>
       </c>
@@ -10698,7 +10701,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="171"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -10723,7 +10726,7 @@
       <c r="I6" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="J6" s="178"/>
+      <c r="J6" s="175"/>
       <c r="L6" s="85" t="s">
         <v>125</v>
       </c>
@@ -10732,7 +10735,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="171"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -10757,10 +10760,10 @@
       <c r="I7" s="15">
         <v>45661</v>
       </c>
-      <c r="J7" s="178"/>
+      <c r="J7" s="175"/>
     </row>
     <row r="8" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="171"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="12">
         <v>6</v>
       </c>
@@ -10785,10 +10788,10 @@
       <c r="I8" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="178"/>
+      <c r="J8" s="175"/>
     </row>
     <row r="9" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -10813,10 +10816,10 @@
       <c r="I9" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="J9" s="178"/>
+      <c r="J9" s="175"/>
     </row>
     <row r="10" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="171"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -10841,10 +10844,10 @@
       <c r="I10" s="53">
         <v>45659</v>
       </c>
-      <c r="J10" s="178"/>
+      <c r="J10" s="175"/>
     </row>
     <row r="11" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="171"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -10869,10 +10872,10 @@
       <c r="I11" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="J11" s="178"/>
+      <c r="J11" s="175"/>
     </row>
     <row r="12" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="171"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -10897,10 +10900,10 @@
       <c r="I12" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="J12" s="178"/>
+      <c r="J12" s="175"/>
     </row>
     <row r="13" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="171"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -10923,10 +10926,10 @@
         <v>150</v>
       </c>
       <c r="I13" s="11"/>
-      <c r="J13" s="178"/>
+      <c r="J13" s="175"/>
     </row>
     <row r="14" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="172"/>
+      <c r="A14" s="168"/>
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -10949,22 +10952,22 @@
         <v>150</v>
       </c>
       <c r="I14" s="14"/>
-      <c r="J14" s="178"/>
+      <c r="J14" s="175"/>
     </row>
     <row r="15" spans="1:13" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="193"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="168"/>
-      <c r="J15" s="178"/>
+      <c r="A15" s="201"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="175"/>
     </row>
     <row r="16" spans="1:13" ht="69" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="166" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -10989,10 +10992,10 @@
         <v>150</v>
       </c>
       <c r="I16" s="56"/>
-      <c r="J16" s="178"/>
+      <c r="J16" s="175"/>
     </row>
     <row r="17" spans="1:10" ht="69" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -11015,19 +11018,19 @@
         <v>150</v>
       </c>
       <c r="I17" s="56"/>
-      <c r="J17" s="178"/>
+      <c r="J17" s="175"/>
     </row>
     <row r="18" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="193"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
-      <c r="J18" s="178"/>
+      <c r="A18" s="201"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
+      <c r="J18" s="175"/>
     </row>
     <row r="19" spans="1:10" ht="69" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -11055,19 +11058,19 @@
         <v>150</v>
       </c>
       <c r="I19" s="102"/>
-      <c r="J19" s="178"/>
+      <c r="J19" s="175"/>
     </row>
     <row r="20" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="193"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
-      <c r="J20" s="178"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="175"/>
     </row>
     <row r="21" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -11095,19 +11098,19 @@
         <v>150</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="178"/>
+      <c r="J21" s="175"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="199"/>
-      <c r="B22" s="178"/>
-      <c r="C22" s="178"/>
-      <c r="D22" s="178"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="178"/>
-      <c r="H22" s="178"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="178"/>
+      <c r="A22" s="200"/>
+      <c r="B22" s="175"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="175"/>
+      <c r="E22" s="175"/>
+      <c r="F22" s="175"/>
+      <c r="G22" s="175"/>
+      <c r="H22" s="175"/>
+      <c r="I22" s="175"/>
+      <c r="J22" s="175"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12364,17 +12367,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:13" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -12406,7 +12409,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="166" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -12720,7 +12723,7 @@
       <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="208"/>
+      <c r="A14" s="204"/>
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -12746,19 +12749,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:13" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="193"/>
-      <c r="B15" s="206"/>
-      <c r="C15" s="206"/>
-      <c r="D15" s="206"/>
-      <c r="E15" s="206"/>
-      <c r="F15" s="206"/>
-      <c r="G15" s="206"/>
-      <c r="H15" s="206"/>
-      <c r="I15" s="207"/>
+      <c r="A15" s="201"/>
+      <c r="B15" s="202"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="202"/>
+      <c r="F15" s="202"/>
+      <c r="G15" s="202"/>
+      <c r="H15" s="202"/>
+      <c r="I15" s="203"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="166" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -12786,7 +12789,7 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="208"/>
+      <c r="A17" s="204"/>
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -12812,15 +12815,15 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="193"/>
-      <c r="B18" s="206"/>
-      <c r="C18" s="206"/>
-      <c r="D18" s="206"/>
-      <c r="E18" s="206"/>
-      <c r="F18" s="206"/>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="207"/>
+      <c r="A18" s="201"/>
+      <c r="B18" s="202"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="202"/>
+      <c r="F18" s="202"/>
+      <c r="G18" s="202"/>
+      <c r="H18" s="202"/>
+      <c r="I18" s="203"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -12852,15 +12855,15 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="193"/>
-      <c r="B20" s="206"/>
-      <c r="C20" s="206"/>
-      <c r="D20" s="206"/>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="207"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="202"/>
+      <c r="C20" s="202"/>
+      <c r="D20" s="202"/>
+      <c r="E20" s="202"/>
+      <c r="F20" s="202"/>
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="203"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -14202,7 +14205,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -14432,7 +14435,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14448,17 +14451,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
     </row>
     <row r="2" spans="1:9" ht="122.4" x14ac:dyDescent="0.3">
       <c r="A2" s="93"/>
@@ -14488,7 +14491,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="205" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="36">
@@ -14517,7 +14520,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="195"/>
+      <c r="A4" s="206"/>
       <c r="B4" s="32">
         <v>2</v>
       </c>
@@ -14544,7 +14547,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="195"/>
+      <c r="A5" s="206"/>
       <c r="B5" s="36">
         <v>3</v>
       </c>
@@ -14571,7 +14574,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="195"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="32">
         <v>4</v>
       </c>
@@ -14598,7 +14601,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="195"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="36">
         <v>5</v>
       </c>
@@ -14625,7 +14628,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="196"/>
+      <c r="A8" s="207"/>
       <c r="B8" s="32">
         <v>6</v>
       </c>
@@ -14653,7 +14656,7 @@
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="166" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="1">
@@ -14680,7 +14683,7 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="172"/>
+      <c r="A11" s="168"/>
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -14705,15 +14708,15 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="193"/>
-      <c r="B12" s="167"/>
-      <c r="C12" s="167"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="167"/>
-      <c r="F12" s="167"/>
-      <c r="G12" s="167"/>
-      <c r="H12" s="167"/>
-      <c r="I12" s="168"/>
+      <c r="A12" s="201"/>
+      <c r="B12" s="182"/>
+      <c r="C12" s="182"/>
+      <c r="D12" s="182"/>
+      <c r="E12" s="182"/>
+      <c r="F12" s="182"/>
+      <c r="G12" s="182"/>
+      <c r="H12" s="182"/>
+      <c r="I12" s="183"/>
     </row>
     <row r="13" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -14743,15 +14746,15 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="193"/>
-      <c r="B14" s="167"/>
-      <c r="C14" s="167"/>
-      <c r="D14" s="167"/>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="168"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="182"/>
+      <c r="C14" s="182"/>
+      <c r="D14" s="182"/>
+      <c r="E14" s="182"/>
+      <c r="F14" s="182"/>
+      <c r="G14" s="182"/>
+      <c r="H14" s="182"/>
+      <c r="I14" s="183"/>
     </row>
     <row r="15" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -15131,17 +15134,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15173,7 +15176,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="166" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -15203,7 +15206,7 @@
       <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="171"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -15231,7 +15234,7 @@
       <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -15259,7 +15262,7 @@
       <c r="J5" s="27"/>
     </row>
     <row r="6" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="171"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -15287,7 +15290,7 @@
       <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="171"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -15315,7 +15318,7 @@
       <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="171"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="12">
         <v>6</v>
       </c>
@@ -15343,7 +15346,7 @@
       <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -15371,7 +15374,7 @@
       <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="171"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -15399,7 +15402,7 @@
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="171"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -15427,7 +15430,7 @@
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="171"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -15453,7 +15456,7 @@
       <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="171"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -15479,7 +15482,7 @@
       <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="172"/>
+      <c r="A14" s="168"/>
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -15505,19 +15508,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="193"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="168"/>
+      <c r="A15" s="201"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="166" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -15545,7 +15548,7 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -15571,15 +15574,15 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="193"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
+      <c r="A18" s="201"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="91.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -15611,15 +15614,15 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="193"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -15927,17 +15930,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:11" ht="61.2" x14ac:dyDescent="0.3">
@@ -15969,7 +15972,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="205" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="32">
@@ -15999,7 +16002,7 @@
       <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="195"/>
+      <c r="A4" s="206"/>
       <c r="B4" s="36">
         <v>2</v>
       </c>
@@ -16028,7 +16031,7 @@
       <c r="K4" s="39"/>
     </row>
     <row r="5" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="195"/>
+      <c r="A5" s="206"/>
       <c r="B5" s="36">
         <v>3</v>
       </c>
@@ -16056,7 +16059,7 @@
       <c r="J5" s="27"/>
     </row>
     <row r="6" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="195"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="32">
         <v>4</v>
       </c>
@@ -16084,7 +16087,7 @@
       <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="195"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="36">
         <v>5</v>
       </c>
@@ -16112,7 +16115,7 @@
       <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:11" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="196"/>
+      <c r="A8" s="207"/>
       <c r="B8" s="32">
         <v>6</v>
       </c>
@@ -16209,19 +16212,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="197"/>
-      <c r="B15" s="181"/>
-      <c r="C15" s="181"/>
-      <c r="D15" s="181"/>
-      <c r="E15" s="181"/>
-      <c r="F15" s="181"/>
-      <c r="G15" s="181"/>
-      <c r="H15" s="181"/>
-      <c r="I15" s="182"/>
+      <c r="A15" s="208"/>
+      <c r="B15" s="178"/>
+      <c r="C15" s="178"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="178"/>
+      <c r="F15" s="178"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="179"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="166" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -16249,7 +16252,7 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -16275,15 +16278,15 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="193"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
+      <c r="A18" s="201"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -16315,15 +16318,15 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="193"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -17376,16 +17379,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="191"/>
-      <c r="B1" s="167"/>
-      <c r="C1" s="168"/>
+      <c r="A1" s="184"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="183"/>
       <c r="D1" s="126" t="s">
         <v>275</v>
       </c>
       <c r="E1" s="126" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="189"/>
+      <c r="F1" s="185"/>
     </row>
     <row r="2" spans="1:6" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28"/>
@@ -17401,13 +17404,13 @@
       <c r="E2" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="F2" s="178"/>
+      <c r="F2" s="175"/>
     </row>
     <row r="3" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="184" t="s">
+      <c r="A3" s="180" t="s">
         <v>307</v>
       </c>
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="180" t="s">
         <v>279</v>
       </c>
       <c r="C3" s="127">
@@ -17419,11 +17422,11 @@
       <c r="E3" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="F3" s="189"/>
+      <c r="F3" s="185"/>
     </row>
     <row r="4" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="177"/>
-      <c r="B4" s="177"/>
+      <c r="A4" s="174"/>
+      <c r="B4" s="174"/>
       <c r="C4" s="129">
         <v>2</v>
       </c>
@@ -17433,11 +17436,11 @@
       <c r="E4" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="F4" s="178"/>
+      <c r="F4" s="175"/>
     </row>
     <row r="5" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="177"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="174"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="129">
         <v>3</v>
       </c>
@@ -17447,11 +17450,11 @@
       <c r="E5" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="F5" s="178"/>
+      <c r="F5" s="175"/>
     </row>
     <row r="6" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="177"/>
-      <c r="B6" s="180"/>
+      <c r="A6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="131">
         <v>4</v>
       </c>
@@ -17461,11 +17464,11 @@
       <c r="E6" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="F6" s="178"/>
+      <c r="F6" s="175"/>
     </row>
     <row r="7" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="177"/>
-      <c r="B7" s="184" t="s">
+      <c r="A7" s="174"/>
+      <c r="B7" s="180" t="s">
         <v>285</v>
       </c>
       <c r="C7" s="127">
@@ -17477,11 +17480,11 @@
       <c r="E7" s="134" t="s">
         <v>317</v>
       </c>
-      <c r="F7" s="178"/>
+      <c r="F7" s="175"/>
     </row>
     <row r="8" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="177"/>
-      <c r="B8" s="177"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="129">
         <v>2</v>
       </c>
@@ -17491,11 +17494,11 @@
       <c r="E8" s="136" t="s">
         <v>309</v>
       </c>
-      <c r="F8" s="178"/>
+      <c r="F8" s="175"/>
     </row>
     <row r="9" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="177"/>
-      <c r="B9" s="177"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="129">
         <v>3</v>
       </c>
@@ -17505,11 +17508,11 @@
       <c r="E9" s="137" t="s">
         <v>320</v>
       </c>
-      <c r="F9" s="178"/>
+      <c r="F9" s="175"/>
     </row>
     <row r="10" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="177"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="174"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="131">
         <v>4</v>
       </c>
@@ -17519,11 +17522,11 @@
       <c r="E10" s="139" t="s">
         <v>322</v>
       </c>
-      <c r="F10" s="178"/>
+      <c r="F10" s="175"/>
     </row>
     <row r="11" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="177"/>
-      <c r="B11" s="180"/>
+      <c r="A11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="131">
         <v>5</v>
       </c>
@@ -17533,11 +17536,11 @@
       <c r="E11" s="139" t="s">
         <v>324</v>
       </c>
-      <c r="F11" s="178"/>
+      <c r="F11" s="175"/>
     </row>
     <row r="12" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="177"/>
-      <c r="B12" s="184" t="s">
+      <c r="A12" s="174"/>
+      <c r="B12" s="180" t="s">
         <v>282</v>
       </c>
       <c r="C12" s="127">
@@ -17549,11 +17552,11 @@
       <c r="E12" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="F12" s="178"/>
+      <c r="F12" s="175"/>
     </row>
     <row r="13" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="177"/>
-      <c r="B13" s="177"/>
+      <c r="A13" s="174"/>
+      <c r="B13" s="174"/>
       <c r="C13" s="129">
         <v>2</v>
       </c>
@@ -17563,11 +17566,11 @@
       <c r="E13" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="F13" s="178"/>
+      <c r="F13" s="175"/>
     </row>
     <row r="14" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="177"/>
-      <c r="B14" s="177"/>
+      <c r="A14" s="174"/>
+      <c r="B14" s="174"/>
       <c r="C14" s="129">
         <v>3</v>
       </c>
@@ -17577,11 +17580,11 @@
       <c r="E14" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="F14" s="178"/>
+      <c r="F14" s="175"/>
     </row>
     <row r="15" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="177"/>
-      <c r="B15" s="177"/>
+      <c r="A15" s="174"/>
+      <c r="B15" s="174"/>
       <c r="C15" s="131">
         <v>4</v>
       </c>
@@ -17591,11 +17594,11 @@
       <c r="E15" s="25" t="s">
         <v>329</v>
       </c>
-      <c r="F15" s="178"/>
+      <c r="F15" s="175"/>
     </row>
     <row r="16" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="177"/>
-      <c r="B16" s="180"/>
+      <c r="A16" s="174"/>
+      <c r="B16" s="177"/>
       <c r="C16" s="131">
         <v>5</v>
       </c>
@@ -17605,11 +17608,11 @@
       <c r="E16" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="F16" s="178"/>
+      <c r="F16" s="175"/>
     </row>
     <row r="17" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="177"/>
-      <c r="B17" s="184" t="s">
+      <c r="A17" s="174"/>
+      <c r="B17" s="180" t="s">
         <v>287</v>
       </c>
       <c r="C17" s="140">
@@ -17618,60 +17621,60 @@
       <c r="D17" s="141" t="s">
         <v>325</v>
       </c>
-      <c r="E17" s="192"/>
-      <c r="F17" s="178"/>
+      <c r="E17" s="186"/>
+      <c r="F17" s="175"/>
     </row>
     <row r="18" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="177"/>
-      <c r="B18" s="177"/>
+      <c r="A18" s="174"/>
+      <c r="B18" s="174"/>
       <c r="C18" s="143">
         <v>2</v>
       </c>
       <c r="D18" s="130" t="s">
         <v>319</v>
       </c>
-      <c r="E18" s="179"/>
-      <c r="F18" s="178"/>
+      <c r="E18" s="176"/>
+      <c r="F18" s="175"/>
     </row>
     <row r="19" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="177"/>
-      <c r="B19" s="177"/>
+      <c r="A19" s="174"/>
+      <c r="B19" s="174"/>
       <c r="C19" s="143">
         <v>3</v>
       </c>
       <c r="D19" s="130" t="s">
         <v>332</v>
       </c>
-      <c r="E19" s="179"/>
-      <c r="F19" s="178"/>
+      <c r="E19" s="176"/>
+      <c r="F19" s="175"/>
     </row>
     <row r="20" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="177"/>
-      <c r="B20" s="177"/>
+      <c r="A20" s="174"/>
+      <c r="B20" s="174"/>
       <c r="C20" s="144">
         <v>4</v>
       </c>
       <c r="D20" s="145" t="s">
         <v>328</v>
       </c>
-      <c r="E20" s="179"/>
-      <c r="F20" s="178"/>
+      <c r="E20" s="176"/>
+      <c r="F20" s="175"/>
     </row>
     <row r="21" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="177"/>
-      <c r="B21" s="180"/>
+      <c r="A21" s="174"/>
+      <c r="B21" s="177"/>
       <c r="C21" s="110">
         <v>5</v>
       </c>
       <c r="D21" s="142" t="s">
         <v>333</v>
       </c>
-      <c r="E21" s="182"/>
-      <c r="F21" s="178"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="175"/>
     </row>
     <row r="22" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="177"/>
-      <c r="B22" s="184" t="s">
+      <c r="A22" s="174"/>
+      <c r="B22" s="180" t="s">
         <v>334</v>
       </c>
       <c r="C22" s="127">
@@ -17681,11 +17684,11 @@
         <v>335</v>
       </c>
       <c r="E22" s="130"/>
-      <c r="F22" s="178"/>
+      <c r="F22" s="175"/>
     </row>
     <row r="23" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="177"/>
-      <c r="B23" s="177"/>
+      <c r="A23" s="174"/>
+      <c r="B23" s="174"/>
       <c r="C23" s="129">
         <v>2</v>
       </c>
@@ -17693,11 +17696,11 @@
         <v>336</v>
       </c>
       <c r="E23" s="146"/>
-      <c r="F23" s="178"/>
+      <c r="F23" s="175"/>
     </row>
     <row r="24" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="177"/>
-      <c r="B24" s="177"/>
+      <c r="A24" s="174"/>
+      <c r="B24" s="174"/>
       <c r="C24" s="129">
         <v>3</v>
       </c>
@@ -17705,11 +17708,11 @@
         <v>95</v>
       </c>
       <c r="E24" s="130"/>
-      <c r="F24" s="178"/>
+      <c r="F24" s="175"/>
     </row>
     <row r="25" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="180"/>
-      <c r="B25" s="180"/>
+      <c r="A25" s="177"/>
+      <c r="B25" s="177"/>
       <c r="C25" s="147">
         <v>4</v>
       </c>
@@ -17717,29 +17720,29 @@
         <v>337</v>
       </c>
       <c r="E25" s="149"/>
-      <c r="F25" s="178"/>
+      <c r="F25" s="175"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="190"/>
-      <c r="B26" s="175"/>
-      <c r="C26" s="175"/>
-      <c r="D26" s="175"/>
-      <c r="E26" s="176"/>
-      <c r="F26" s="178"/>
+      <c r="A26" s="187"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="172"/>
+      <c r="D26" s="172"/>
+      <c r="E26" s="173"/>
+      <c r="F26" s="175"/>
     </row>
     <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="180"/>
-      <c r="B27" s="181"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="178"/>
+      <c r="A27" s="177"/>
+      <c r="B27" s="178"/>
+      <c r="C27" s="178"/>
+      <c r="D27" s="178"/>
+      <c r="E27" s="179"/>
+      <c r="F27" s="175"/>
     </row>
     <row r="28" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="173" t="s">
+      <c r="A28" s="166" t="s">
         <v>288</v>
       </c>
-      <c r="B28" s="173" t="s">
+      <c r="B28" s="166" t="s">
         <v>279</v>
       </c>
       <c r="C28" s="1">
@@ -17751,11 +17754,11 @@
       <c r="E28" s="150" t="s">
         <v>339</v>
       </c>
-      <c r="F28" s="178"/>
+      <c r="F28" s="175"/>
     </row>
     <row r="29" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="171"/>
-      <c r="B29" s="171"/>
+      <c r="A29" s="167"/>
+      <c r="B29" s="167"/>
       <c r="C29" s="1">
         <v>2</v>
       </c>
@@ -17765,11 +17768,11 @@
       <c r="E29" s="150" t="s">
         <v>341</v>
       </c>
-      <c r="F29" s="178"/>
+      <c r="F29" s="175"/>
     </row>
     <row r="30" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="171"/>
-      <c r="B30" s="171"/>
+      <c r="A30" s="167"/>
+      <c r="B30" s="167"/>
       <c r="C30" s="1">
         <v>3</v>
       </c>
@@ -17779,11 +17782,11 @@
       <c r="E30" s="150" t="s">
         <v>315</v>
       </c>
-      <c r="F30" s="178"/>
+      <c r="F30" s="175"/>
     </row>
     <row r="31" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="171"/>
-      <c r="B31" s="172"/>
+      <c r="A31" s="167"/>
+      <c r="B31" s="168"/>
       <c r="C31" s="1">
         <v>4</v>
       </c>
@@ -17793,11 +17796,11 @@
       <c r="E31" s="150" t="s">
         <v>313</v>
       </c>
-      <c r="F31" s="178"/>
+      <c r="F31" s="175"/>
     </row>
     <row r="32" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="171"/>
-      <c r="B32" s="173" t="s">
+      <c r="A32" s="167"/>
+      <c r="B32" s="166" t="s">
         <v>285</v>
       </c>
       <c r="C32" s="1">
@@ -17809,11 +17812,11 @@
       <c r="E32" s="150" t="s">
         <v>345</v>
       </c>
-      <c r="F32" s="178"/>
+      <c r="F32" s="175"/>
     </row>
     <row r="33" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="171"/>
-      <c r="B33" s="171"/>
+      <c r="A33" s="167"/>
+      <c r="B33" s="167"/>
       <c r="C33" s="1">
         <v>2</v>
       </c>
@@ -17823,11 +17826,11 @@
       <c r="E33" s="150" t="s">
         <v>347</v>
       </c>
-      <c r="F33" s="178"/>
+      <c r="F33" s="175"/>
     </row>
     <row r="34" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="171"/>
-      <c r="B34" s="171"/>
+      <c r="A34" s="167"/>
+      <c r="B34" s="167"/>
       <c r="C34" s="1">
         <v>3</v>
       </c>
@@ -17837,11 +17840,11 @@
       <c r="E34" s="150" t="s">
         <v>349</v>
       </c>
-      <c r="F34" s="178"/>
+      <c r="F34" s="175"/>
     </row>
     <row r="35" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="171"/>
-      <c r="B35" s="172"/>
+      <c r="A35" s="167"/>
+      <c r="B35" s="168"/>
       <c r="C35" s="1">
         <v>4</v>
       </c>
@@ -17849,11 +17852,11 @@
         <v>350</v>
       </c>
       <c r="E35" s="150"/>
-      <c r="F35" s="178"/>
+      <c r="F35" s="175"/>
     </row>
     <row r="36" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="171"/>
-      <c r="B36" s="173" t="s">
+      <c r="A36" s="167"/>
+      <c r="B36" s="166" t="s">
         <v>282</v>
       </c>
       <c r="C36" s="1">
@@ -17865,11 +17868,11 @@
       <c r="E36" s="150" t="s">
         <v>351</v>
       </c>
-      <c r="F36" s="178"/>
+      <c r="F36" s="175"/>
     </row>
     <row r="37" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="171"/>
-      <c r="B37" s="171"/>
+      <c r="A37" s="167"/>
+      <c r="B37" s="167"/>
       <c r="C37" s="1">
         <v>2</v>
       </c>
@@ -17879,11 +17882,11 @@
       <c r="E37" s="150" t="s">
         <v>353</v>
       </c>
-      <c r="F37" s="178"/>
+      <c r="F37" s="175"/>
     </row>
     <row r="38" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="171"/>
-      <c r="B38" s="171"/>
+      <c r="A38" s="167"/>
+      <c r="B38" s="167"/>
       <c r="C38" s="1">
         <v>3</v>
       </c>
@@ -17893,11 +17896,11 @@
       <c r="E38" s="150" t="s">
         <v>355</v>
       </c>
-      <c r="F38" s="178"/>
+      <c r="F38" s="175"/>
     </row>
     <row r="39" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="171"/>
-      <c r="B39" s="171"/>
+      <c r="A39" s="167"/>
+      <c r="B39" s="167"/>
       <c r="C39" s="1">
         <v>4</v>
       </c>
@@ -17907,21 +17910,21 @@
       <c r="E39" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="F39" s="178"/>
+      <c r="F39" s="175"/>
     </row>
     <row r="40" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="171"/>
-      <c r="B40" s="172"/>
+      <c r="A40" s="167"/>
+      <c r="B40" s="168"/>
       <c r="C40" s="1">
         <v>5</v>
       </c>
       <c r="D40" s="150"/>
       <c r="E40" s="150"/>
-      <c r="F40" s="178"/>
+      <c r="F40" s="175"/>
     </row>
     <row r="41" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="171"/>
-      <c r="B41" s="173" t="s">
+      <c r="A41" s="167"/>
+      <c r="B41" s="166" t="s">
         <v>287</v>
       </c>
       <c r="C41" s="1">
@@ -17930,48 +17933,48 @@
       <c r="D41" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="E41" s="187"/>
-      <c r="F41" s="178"/>
+      <c r="E41" s="188"/>
+      <c r="F41" s="175"/>
     </row>
     <row r="42" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="171"/>
-      <c r="B42" s="171"/>
+      <c r="A42" s="167"/>
+      <c r="B42" s="167"/>
       <c r="C42" s="1">
         <v>2</v>
       </c>
       <c r="D42" s="150" t="s">
         <v>308</v>
       </c>
-      <c r="E42" s="171"/>
-      <c r="F42" s="178"/>
+      <c r="E42" s="167"/>
+      <c r="F42" s="175"/>
     </row>
     <row r="43" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="171"/>
-      <c r="B43" s="171"/>
+      <c r="A43" s="167"/>
+      <c r="B43" s="167"/>
       <c r="C43" s="1">
         <v>3</v>
       </c>
       <c r="D43" s="150" t="s">
         <v>358</v>
       </c>
-      <c r="E43" s="171"/>
-      <c r="F43" s="178"/>
+      <c r="E43" s="167"/>
+      <c r="F43" s="175"/>
     </row>
     <row r="44" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="171"/>
-      <c r="B44" s="172"/>
+      <c r="A44" s="167"/>
+      <c r="B44" s="168"/>
       <c r="C44" s="1">
         <v>4</v>
       </c>
       <c r="D44" s="150" t="s">
         <v>359</v>
       </c>
-      <c r="E44" s="172"/>
-      <c r="F44" s="178"/>
+      <c r="E44" s="168"/>
+      <c r="F44" s="175"/>
     </row>
     <row r="45" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="171"/>
-      <c r="B45" s="173" t="s">
+      <c r="A45" s="167"/>
+      <c r="B45" s="166" t="s">
         <v>334</v>
       </c>
       <c r="C45" s="1">
@@ -17983,11 +17986,11 @@
       <c r="E45" s="150" t="s">
         <v>336</v>
       </c>
-      <c r="F45" s="178"/>
+      <c r="F45" s="175"/>
     </row>
     <row r="46" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="171"/>
-      <c r="B46" s="171"/>
+      <c r="A46" s="167"/>
+      <c r="B46" s="167"/>
       <c r="C46" s="1">
         <v>2</v>
       </c>
@@ -17997,11 +18000,11 @@
       <c r="E46" s="150" t="s">
         <v>337</v>
       </c>
-      <c r="F46" s="178"/>
+      <c r="F46" s="175"/>
     </row>
     <row r="47" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="171"/>
-      <c r="B47" s="171"/>
+      <c r="A47" s="167"/>
+      <c r="B47" s="167"/>
       <c r="C47" s="1">
         <v>3</v>
       </c>
@@ -18011,11 +18014,11 @@
       <c r="E47" s="150" t="s">
         <v>95</v>
       </c>
-      <c r="F47" s="178"/>
+      <c r="F47" s="175"/>
     </row>
     <row r="48" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="171"/>
-      <c r="B48" s="172"/>
+      <c r="A48" s="167"/>
+      <c r="B48" s="168"/>
       <c r="C48" s="1">
         <v>4</v>
       </c>
@@ -18023,11 +18026,11 @@
       <c r="E48" s="150" t="s">
         <v>335</v>
       </c>
-      <c r="F48" s="178"/>
+      <c r="F48" s="175"/>
     </row>
     <row r="49" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="171"/>
-      <c r="B49" s="173" t="s">
+      <c r="A49" s="167"/>
+      <c r="B49" s="166" t="s">
         <v>361</v>
       </c>
       <c r="C49" s="1">
@@ -18036,36 +18039,36 @@
       <c r="D49" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="E49" s="187"/>
-      <c r="F49" s="178"/>
+      <c r="E49" s="188"/>
+      <c r="F49" s="175"/>
     </row>
     <row r="50" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="171"/>
-      <c r="B50" s="171"/>
+      <c r="A50" s="167"/>
+      <c r="B50" s="167"/>
       <c r="C50" s="1">
         <v>2</v>
       </c>
       <c r="D50" s="24" t="s">
         <v>363</v>
       </c>
-      <c r="E50" s="171"/>
-      <c r="F50" s="178"/>
+      <c r="E50" s="167"/>
+      <c r="F50" s="175"/>
     </row>
     <row r="51" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="171"/>
-      <c r="B51" s="172"/>
+      <c r="A51" s="167"/>
+      <c r="B51" s="168"/>
       <c r="C51" s="1">
         <v>3</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>364</v>
       </c>
-      <c r="E51" s="171"/>
-      <c r="F51" s="178"/>
+      <c r="E51" s="167"/>
+      <c r="F51" s="175"/>
     </row>
     <row r="52" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="171"/>
-      <c r="B52" s="173" t="s">
+      <c r="A52" s="167"/>
+      <c r="B52" s="166" t="s">
         <v>365</v>
       </c>
       <c r="C52" s="1">
@@ -18074,36 +18077,36 @@
       <c r="D52" s="151" t="s">
         <v>366</v>
       </c>
-      <c r="E52" s="171"/>
-      <c r="F52" s="178"/>
+      <c r="E52" s="167"/>
+      <c r="F52" s="175"/>
     </row>
     <row r="53" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="171"/>
-      <c r="B53" s="171"/>
+      <c r="A53" s="167"/>
+      <c r="B53" s="167"/>
       <c r="C53" s="1">
         <v>2</v>
       </c>
       <c r="D53" s="151" t="s">
         <v>367</v>
       </c>
-      <c r="E53" s="171"/>
-      <c r="F53" s="178"/>
+      <c r="E53" s="167"/>
+      <c r="F53" s="175"/>
     </row>
     <row r="54" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="171"/>
-      <c r="B54" s="172"/>
+      <c r="A54" s="167"/>
+      <c r="B54" s="168"/>
       <c r="C54" s="1">
         <v>3</v>
       </c>
       <c r="D54" s="151" t="s">
         <v>364</v>
       </c>
-      <c r="E54" s="172"/>
-      <c r="F54" s="178"/>
+      <c r="E54" s="168"/>
+      <c r="F54" s="175"/>
     </row>
     <row r="55" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="171"/>
-      <c r="B55" s="173" t="s">
+      <c r="A55" s="167"/>
+      <c r="B55" s="166" t="s">
         <v>368</v>
       </c>
       <c r="C55" s="1">
@@ -18115,11 +18118,11 @@
       <c r="E55" s="151" t="s">
         <v>369</v>
       </c>
-      <c r="F55" s="178"/>
+      <c r="F55" s="175"/>
     </row>
     <row r="56" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="171"/>
-      <c r="B56" s="171"/>
+      <c r="A56" s="167"/>
+      <c r="B56" s="167"/>
       <c r="C56" s="1">
         <v>2</v>
       </c>
@@ -18129,11 +18132,11 @@
       <c r="E56" s="151" t="s">
         <v>370</v>
       </c>
-      <c r="F56" s="178"/>
+      <c r="F56" s="175"/>
     </row>
     <row r="57" spans="1:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="171"/>
-      <c r="B57" s="171"/>
+      <c r="A57" s="167"/>
+      <c r="B57" s="167"/>
       <c r="C57" s="1">
         <v>3</v>
       </c>
@@ -18143,11 +18146,11 @@
       <c r="E57" s="151" t="s">
         <v>371</v>
       </c>
-      <c r="F57" s="178"/>
+      <c r="F57" s="175"/>
     </row>
     <row r="58" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="171"/>
-      <c r="B58" s="173" t="s">
+      <c r="A58" s="167"/>
+      <c r="B58" s="166" t="s">
         <v>304</v>
       </c>
       <c r="C58" s="1">
@@ -18156,60 +18159,60 @@
       <c r="D58" s="24" t="s">
         <v>372</v>
       </c>
-      <c r="E58" s="187"/>
-      <c r="F58" s="178"/>
+      <c r="E58" s="188"/>
+      <c r="F58" s="175"/>
     </row>
     <row r="59" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="171"/>
-      <c r="B59" s="171"/>
+      <c r="A59" s="167"/>
+      <c r="B59" s="167"/>
       <c r="C59" s="1">
         <v>2</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>373</v>
       </c>
-      <c r="E59" s="171"/>
-      <c r="F59" s="178"/>
+      <c r="E59" s="167"/>
+      <c r="F59" s="175"/>
     </row>
     <row r="60" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="171"/>
-      <c r="B60" s="171"/>
+      <c r="A60" s="167"/>
+      <c r="B60" s="167"/>
       <c r="C60" s="1">
         <v>3</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="E60" s="171"/>
-      <c r="F60" s="178"/>
+      <c r="E60" s="167"/>
+      <c r="F60" s="175"/>
     </row>
     <row r="61" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="172"/>
-      <c r="B61" s="172"/>
+      <c r="A61" s="168"/>
+      <c r="B61" s="168"/>
       <c r="C61" s="1">
         <v>4</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="E61" s="172"/>
-      <c r="F61" s="178"/>
+      <c r="E61" s="168"/>
+      <c r="F61" s="175"/>
     </row>
     <row r="62" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="188"/>
-      <c r="B62" s="167"/>
-      <c r="C62" s="167"/>
-      <c r="D62" s="167"/>
-      <c r="E62" s="168"/>
-      <c r="F62" s="178"/>
+      <c r="A62" s="189"/>
+      <c r="B62" s="182"/>
+      <c r="C62" s="182"/>
+      <c r="D62" s="182"/>
+      <c r="E62" s="183"/>
+      <c r="F62" s="175"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="189"/>
-      <c r="B63" s="178"/>
-      <c r="C63" s="178"/>
-      <c r="D63" s="178"/>
-      <c r="E63" s="178"/>
-      <c r="F63" s="178"/>
+      <c r="A63" s="185"/>
+      <c r="B63" s="175"/>
+      <c r="C63" s="175"/>
+      <c r="D63" s="175"/>
+      <c r="E63" s="175"/>
+      <c r="F63" s="175"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -19103,16 +19106,6 @@
     <row r="953" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:A25"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="F3:F62"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="B22:B25"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A26:E27"/>
     <mergeCell ref="A28:A61"/>
@@ -19129,6 +19122,16 @@
     <mergeCell ref="B58:B61"/>
     <mergeCell ref="E58:E61"/>
     <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A25"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="F3:F62"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="B22:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19388,17 +19391,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="191" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:14" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -19430,7 +19433,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="192" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -19460,7 +19463,7 @@
       <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="171"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -19489,7 +19492,7 @@
       <c r="L4" s="48"/>
     </row>
     <row r="5" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="107">
         <v>3</v>
       </c>
@@ -19519,7 +19522,7 @@
       <c r="L5" s="115"/>
     </row>
     <row r="6" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="171"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -19555,7 +19558,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="171"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -19591,7 +19594,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="171"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -19619,7 +19622,7 @@
       <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -19647,7 +19650,7 @@
       <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="171"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -19676,7 +19679,7 @@
       <c r="K10" s="71"/>
     </row>
     <row r="11" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="171"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -19705,7 +19708,7 @@
       <c r="L11" s="71"/>
     </row>
     <row r="12" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="171"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -19734,7 +19737,7 @@
       <c r="L12" s="71"/>
     </row>
     <row r="13" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="171"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -19762,7 +19765,7 @@
       <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:14" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="172"/>
+      <c r="A14" s="168"/>
       <c r="B14" s="7">
         <v>12</v>
       </c>
@@ -19788,19 +19791,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:14" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="166"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="168"/>
+      <c r="A15" s="190"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:14" ht="69" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="193" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -19828,7 +19831,7 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -19854,15 +19857,15 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="166"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
+      <c r="A18" s="190"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -19894,15 +19897,15 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="166"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
+      <c r="A20" s="190"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="69" thickBot="1" x14ac:dyDescent="0.35">
@@ -21203,17 +21206,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="191" t="s">
         <v>255</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:13" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -21245,7 +21248,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="170" t="s">
+      <c r="A3" s="193" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -21275,7 +21278,7 @@
       <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="171"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -21304,7 +21307,7 @@
       <c r="K4" s="48"/>
     </row>
     <row r="5" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -21333,7 +21336,7 @@
       <c r="K5" s="48"/>
     </row>
     <row r="6" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="171"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -21362,7 +21365,7 @@
       <c r="K6" s="48"/>
     </row>
     <row r="7" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="171"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -21391,7 +21394,7 @@
       <c r="K7" s="48"/>
     </row>
     <row r="8" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="171"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -21426,7 +21429,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -21460,7 +21463,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="171"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -21488,7 +21491,7 @@
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="171"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -21514,7 +21517,7 @@
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="172"/>
+      <c r="A12" s="168"/>
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -21564,19 +21567,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:13" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="205"/>
-      <c r="B15" s="181"/>
-      <c r="C15" s="181"/>
-      <c r="D15" s="181"/>
-      <c r="E15" s="181"/>
-      <c r="F15" s="181"/>
-      <c r="G15" s="181"/>
-      <c r="H15" s="181"/>
-      <c r="I15" s="182"/>
+      <c r="A15" s="194"/>
+      <c r="B15" s="178"/>
+      <c r="C15" s="178"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="178"/>
+      <c r="F15" s="178"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="179"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="193" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -21603,7 +21606,7 @@
       <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -21628,15 +21631,15 @@
       <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="166"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
+      <c r="A18" s="190"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
     </row>
     <row r="19" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="s">
@@ -21666,15 +21669,15 @@
       <c r="I19" s="56"/>
     </row>
     <row r="20" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="166"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
+      <c r="A20" s="190"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
     </row>
     <row r="21" spans="1:9" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="24" t="s">
@@ -23007,17 +23010,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="195" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="168"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="183"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:16" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -23049,7 +23052,7 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="170" t="s">
+      <c r="A3" s="193" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7">
@@ -23079,7 +23082,7 @@
       <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="171"/>
+      <c r="A4" s="167"/>
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -23113,7 +23116,7 @@
       <c r="P4" s="39"/>
     </row>
     <row r="5" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="171"/>
+      <c r="A5" s="167"/>
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -23141,7 +23144,7 @@
       <c r="J5" s="27"/>
     </row>
     <row r="6" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="171"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -23168,7 +23171,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="171"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -23196,7 +23199,7 @@
       <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:16" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="171"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="12">
         <v>6</v>
       </c>
@@ -23227,7 +23230,7 @@
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="171"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -23255,7 +23258,7 @@
       <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:16" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="171"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -23283,7 +23286,7 @@
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="171"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -23311,7 +23314,7 @@
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="171"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -23339,7 +23342,7 @@
       <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="171"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -23367,7 +23370,7 @@
       <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="172"/>
+      <c r="A14" s="168"/>
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -23393,19 +23396,19 @@
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="166"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="168"/>
+      <c r="A15" s="190"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="183"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="193" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1">
@@ -23433,7 +23436,7 @@
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="172"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -23459,15 +23462,15 @@
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="166"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
+      <c r="A18" s="190"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="183"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -23499,15 +23502,15 @@
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="166"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="167"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="167"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
+      <c r="A20" s="190"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>